<commit_message>
New configuration file + no printing dataframes + documentation
</commit_message>
<xml_diff>
--- a/jade/default_settings/Config.xlsx
+++ b/jade/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\avalenti\lukas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\jade\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3F7828-7D11-4C92-8D1F-4539B53EA7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D2B8DD-D202-4B4E-84A6-D7AA9EAF2538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="930" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="88">
   <si>
     <t>Suffix</t>
   </si>
@@ -345,7 +345,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,12 +355,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -486,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -494,12 +488,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -560,6 +552,9 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,12 +583,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -909,101 +898,101 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5703125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="20" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="21"/>
     </row>
     <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="B11" s="21"/>
+    </row>
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="B12" s="21"/>
+    </row>
+    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1020,281 +1009,293 @@
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>10000</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="C5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>50000000</v>
       </c>
-      <c r="J5" s="16"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="9" t="s">
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>10000000</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <v>10000000</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="C8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="8">
         <v>100000000</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="37" t="s">
+      <c r="C9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="H9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="8">
         <v>500000000</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="10">
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="8">
         <v>100000000</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1312,434 +1313,440 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="34"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="8">
         <v>10000000</v>
       </c>
-      <c r="J4" s="9"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="C5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="8">
         <v>500000000</v>
       </c>
-      <c r="J5" s="9"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="C6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="8">
         <v>100</v>
       </c>
-      <c r="J6" s="9"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="10">
+      <c r="C7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="8">
         <v>100</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="C8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="8">
         <v>100</v>
       </c>
-      <c r="J8" s="9"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="C9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="8">
         <v>100</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="10">
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="8">
         <v>100</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="10">
+      <c r="C11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="8">
         <v>100</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="10">
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="8">
         <v>100</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="10">
+      <c r="C13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="8">
         <v>100</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="10">
+      <c r="C14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="8">
         <v>100</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="10">
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="8">
         <v>100</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1761,12 +1768,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="64.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1799,15 +1806,12 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1816,11 +1820,6 @@
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1829,11 +1828,6 @@
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1842,11 +1836,6 @@
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1855,11 +1844,6 @@
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1868,13 +1852,9 @@
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tests for tiaraoutputs and shielding output
</commit_message>
<xml_diff>
--- a/jade/default_settings/Config.xlsx
+++ b/jade/default_settings/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\jade\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B34CF9-051B-4BCC-AA54-2308923EC0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A1B0C4-0C96-4074-BDE8-16CAA089C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="90">
   <si>
     <t>Suffix</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>Batch file</t>
+  </si>
+  <si>
+    <t>34y</t>
+  </si>
+  <si>
+    <t>IRDFF-II</t>
   </si>
 </sst>
 </file>
@@ -1766,10 +1772,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,6 +1865,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated job script template, update main config to include MPI exec prefix
</commit_message>
<xml_diff>
--- a/jade/default_settings/Config.xlsx
+++ b/jade/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\jade\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbradnam\AppData\Local\Temp\scp20607\lustre\home\sbradnam\projects\epsrc\benchmarking\software\JADE\Code\jade\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A1B0C4-0C96-4074-BDE8-16CAA089C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1DC350-8DD5-4E7C-9B47-BE3399C30CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="91">
   <si>
     <t>Suffix</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>IRDFF-II</t>
+  </si>
+  <si>
+    <t>MPI executable prefix</t>
   </si>
 </sst>
 </file>
@@ -896,10 +899,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,17 +995,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="21"/>
+    </row>
+    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="21"/>
-    </row>
-    <row r="13" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="B13" s="21"/>
+    </row>
+    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1774,7 +1783,7 @@
   </sheetPr>
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add files for 93c support
</commit_message>
<xml_diff>
--- a/jade/default_settings/Config.xlsx
+++ b/jade/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\jade\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\JADE\Code\jade\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85AEEE0-EAAF-422F-B149-F61E582A871A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B858AE16-F30E-4D5F-BD59-0003F1A8EECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="1515" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="96">
   <si>
     <t>Suffix</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t>Batch file</t>
+  </si>
+  <si>
+    <t>99c</t>
+  </si>
+  <si>
+    <t>D1SUNED (FENDL 3.1d+EAF2007)</t>
+  </si>
+  <si>
+    <t>93c</t>
+  </si>
+  <si>
+    <t>D1SUNED (FENDL 3.2b+DECAY2020)</t>
   </si>
 </sst>
 </file>
@@ -913,19 +925,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.54296875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="25" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
         <v>72</v>
       </c>
@@ -933,7 +945,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>74</v>
       </c>
@@ -941,7 +953,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>76</v>
       </c>
@@ -949,7 +961,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>78</v>
       </c>
@@ -957,7 +969,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
         <v>80</v>
       </c>
@@ -965,7 +977,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="22" t="s">
         <v>82</v>
       </c>
@@ -973,7 +985,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="22" t="s">
         <v>84</v>
       </c>
@@ -981,7 +993,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="22" t="s">
         <v>85</v>
       </c>
@@ -989,7 +1001,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="22" t="s">
         <v>87</v>
       </c>
@@ -997,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="22" t="s">
         <v>88</v>
       </c>
@@ -1005,19 +1017,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B13" s="21"/>
     </row>
-    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
         <v>91</v>
       </c>
@@ -1042,19 +1054,19 @@
       <selection activeCell="I3" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="27" t="s">
         <v>56</v>
       </c>
@@ -1068,7 +1080,7 @@
       <c r="I1" s="29"/>
       <c r="J1" s="30"/>
     </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="31" t="s">
         <v>23</v>
       </c>
@@ -1082,7 +1094,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -1114,7 +1126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>57</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>59</v>
       </c>
@@ -1176,7 +1188,7 @@
       </c>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>61</v>
       </c>
@@ -1206,7 +1218,7 @@
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>63</v>
       </c>
@@ -1236,7 +1248,7 @@
       </c>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>65</v>
       </c>
@@ -1266,7 +1278,7 @@
       </c>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>67</v>
       </c>
@@ -1296,7 +1308,7 @@
       </c>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>69</v>
       </c>
@@ -1342,22 +1354,22 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.54296875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +1383,7 @@
       <c r="I1" s="29"/>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="32" t="s">
         <v>23</v>
       </c>
@@ -1385,7 +1397,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="32"/>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1447,7 +1459,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
@@ -1477,7 +1489,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1507,7 +1519,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -1537,7 +1549,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -1567,7 +1579,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -1597,7 +1609,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1627,7 +1639,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -1657,7 +1669,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1687,7 +1699,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>50</v>
       </c>
@@ -1717,7 +1729,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1759,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>54</v>
       </c>
@@ -1791,21 +1803,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.08984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1828,7 +1842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1836,7 +1850,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1844,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1852,7 +1866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1860,7 +1874,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1868,7 +1882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1879,12 +1893,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add bmark to config
</commit_message>
<xml_diff>
--- a/jade/default_settings/Config.xlsx
+++ b/jade/default_settings/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\JADE\Code\jade\default_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avalenti\AppData\Local\Temp\scp20465\lustre\home\avalenti\JADE\Code\jade\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B858AE16-F30E-4D5F-BD59-0003F1A8EECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389DC4C9-CB37-4FF9-AEBB-823E946AC73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40530" yWindow="2490" windowWidth="23655" windowHeight="17835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="98">
   <si>
     <t>Suffix</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>D1SUNED (FENDL 3.2b+DECAY2020)</t>
+  </si>
+  <si>
+    <t>Simple_Tokamak</t>
+  </si>
+  <si>
+    <t>Simple Tokamak benchmark</t>
   </si>
 </sst>
 </file>
@@ -925,19 +931,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5703125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="25" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="26"/>
     </row>
-    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>72</v>
       </c>
@@ -945,7 +951,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>74</v>
       </c>
@@ -953,7 +959,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>76</v>
       </c>
@@ -961,7 +967,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>78</v>
       </c>
@@ -969,7 +975,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>80</v>
       </c>
@@ -977,7 +983,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>82</v>
       </c>
@@ -985,7 +991,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>84</v>
       </c>
@@ -993,7 +999,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>85</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>87</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>88</v>
       </c>
@@ -1017,19 +1023,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="21"/>
     </row>
-    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B13" s="21"/>
     </row>
-    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>91</v>
       </c>
@@ -1048,25 +1054,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="13.7265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="27" t="s">
         <v>56</v>
       </c>
@@ -1080,7 +1086,7 @@
       <c r="I1" s="29"/>
       <c r="J1" s="30"/>
     </row>
-    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>23</v>
       </c>
@@ -1094,7 +1100,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="34"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>57</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>59</v>
       </c>
@@ -1188,7 +1194,7 @@
       </c>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>61</v>
       </c>
@@ -1218,7 +1224,7 @@
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>63</v>
       </c>
@@ -1248,7 +1254,7 @@
       </c>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>65</v>
       </c>
@@ -1278,7 +1284,7 @@
       </c>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>67</v>
       </c>
@@ -1308,7 +1314,7 @@
       </c>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>69</v>
       </c>
@@ -1337,6 +1343,35 @@
         <v>100000000</v>
       </c>
       <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="10">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1358,18 +1393,18 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.453125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.54296875" style="10" customWidth="1"/>
-    <col min="10" max="10" width="13.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="28" t="s">
         <v>22</v>
       </c>
@@ -1383,7 +1418,7 @@
       <c r="I1" s="29"/>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>23</v>
       </c>
@@ -1397,7 +1432,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="32"/>
     </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -1429,7 +1464,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -1459,7 +1494,7 @@
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
@@ -1489,7 +1524,7 @@
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1519,7 +1554,7 @@
       </c>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
@@ -1549,7 +1584,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -1579,7 +1614,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -1609,7 +1644,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1639,7 +1674,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -1669,7 +1704,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
@@ -1699,7 +1734,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>50</v>
       </c>
@@ -1729,7 +1764,7 @@
       </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>52</v>
       </c>
@@ -1759,7 +1794,7 @@
       </c>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>54</v>
       </c>
@@ -1805,21 +1840,21 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.08984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="64.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1842,7 +1877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1850,7 +1885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1858,7 +1893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1866,7 +1901,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1874,7 +1909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1882,7 +1917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1893,7 +1928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -1901,7 +1936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>92</v>
       </c>
@@ -1909,7 +1944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>94</v>
       </c>

</xml_diff>